<commit_message>
update version of Ellithium
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Scope Assessment1.xlsx
+++ b/src/test/resources/TestData/Scope Assessment1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Item Name</t>
   </si>
@@ -20,34 +20,43 @@
     <t>ItemPrice</t>
   </si>
   <si>
-    <t>Lenovo Gaming Monitor G27c-30 27",1500R Curved Monitor, FHD 1920x1080 Vertical Alignment Display, 16.7 Mn Colors, 165Hz Refresh Rate, 1ms Response Time, AMD FreeSync, 2x HDMI 2.0, 1x DP 1.4</t>
-  </si>
-  <si>
-    <t>11,016</t>
-  </si>
-  <si>
-    <t>ViewSonic Omni VX2728J IPS, 180HZ, 0.5ms</t>
-  </si>
-  <si>
-    <t>11,583</t>
-  </si>
-  <si>
-    <t>ViewSonic Omni VX2428J IPS, 180HZ, 0.5ms</t>
-  </si>
-  <si>
-    <t>8,783</t>
-  </si>
-  <si>
-    <t>Viewsonic Va2710-Mh 27" Monitor Full Hd Ips Panel Hdmi Speaker Black</t>
-  </si>
-  <si>
-    <t>7,999</t>
+    <t>Lenovo Monitor Legion R27fc-30 Gaming Curved Monitor, 27" FHD VA Display, Up to 280Hz Refresh Rate, 0.5ms (MPRT) Response Time, 1500R Curvature, FreeSync, Adaptive Sync &amp; G-Sync Compatible, Black</t>
+  </si>
+  <si>
+    <t>11,999</t>
+  </si>
+  <si>
+    <t>Samsung 27-Inch G55C Odyssey QHD 2K Curved Gaming Monitor, HRDR 10, VA Panel, 1ms MPRT, 165hz with Game Mode, Supports AMD FreeSync, HDMI and DisplayPort, 3 Years Local Warranty</t>
+  </si>
+  <si>
+    <t>7,645</t>
+  </si>
+  <si>
+    <t>Samsung 32-Inch QLED G8 Odyssey Gaming Monitor, with 1ms GtG Response time &amp; 240Hz Refresh rate, Supports AMD FreeSync Premium Pro, Local Warranty</t>
+  </si>
+  <si>
+    <t>82,678</t>
+  </si>
+  <si>
+    <t>Samsung 27-Inch VA Gaming Monitor, 4ms GtG, 60hz with Game Mode, Supports AMD FreeSync, Local Warranty.</t>
+  </si>
+  <si>
+    <t>6,666</t>
   </si>
   <si>
     <t>Samsung 22-Inch IPS Gaming Monitor with Borderless Design, VGA and HDMI, 5ms GtG, 75hz with Game Mode, Supports AMD FreeSync, Local Warranty.</t>
   </si>
   <si>
     <t>3,200</t>
+  </si>
+  <si>
+    <t>12,528</t>
+  </si>
+  <si>
+    <t>12,555</t>
+  </si>
+  <si>
+    <t>9,299</t>
   </si>
 </sst>
 </file>
@@ -92,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -146,6 +155,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>